<commit_message>
AMS Trend inventory fix + data snapshot updates
</commit_message>
<xml_diff>
--- a/data/ams_weekly_data/Audio_Array/business_report_week4.xlsx
+++ b/data/ams_weekly_data/Audio_Array/business_report_week4.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My Laptop\D\Nitesh\Weekly Report - B2B + B2C\FastAPI\data\ams_weekly_data\Audio_Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3A999E-741F-407C-BD07-D3BDAAE0CB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8708E7-9C98-48DF-B4B1-282C0DACA1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{64FFF188-13B2-4234-BE60-38D8C5F3460E}"/>
   </bookViews>
   <sheets>
     <sheet name="amazon_sales" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2256,11 +2267,13 @@
   <dimension ref="A1:W164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Amazon + 1P Sales Trend update
</commit_message>
<xml_diff>
--- a/data/ams_weekly_data/Audio_Array/business_report_week4.xlsx
+++ b/data/ams_weekly_data/Audio_Array/business_report_week4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My Laptop\D\Nitesh\Weekly Report - B2B + B2C\FastAPI\data\ams_weekly_data\Audio_Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8708E7-9C98-48DF-B4B1-282C0DACA1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151D4DF5-3DF3-4366-9F58-D2EB2BB33B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{64FFF188-13B2-4234-BE60-38D8C5F3460E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="465">
   <si>
     <t>SKU</t>
   </si>
@@ -1417,6 +1417,15 @@
   </si>
   <si>
     <t>Audio Array AM-W21 Wireless Microphone Kit | Built in Recording, Noise Reduction &amp; Echo | Smartphones, Cameras, Laptops | Dual-Channel Recording, 200 feet Transmission Range, 48-Hour Battery Life</t>
+  </si>
+  <si>
+    <t>FBA79844</t>
+  </si>
+  <si>
+    <t>PB-08 (AM-C1 + AI-04)</t>
+  </si>
+  <si>
+    <t>B0FN7DYB2M</t>
   </si>
 </sst>
 </file>
@@ -2264,10 +2273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71D4132A-6B30-4EB0-AB5F-9D4A6FCE4FA0}">
-  <dimension ref="A1:W164"/>
+  <dimension ref="A1:W243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13921,6 +13930,1586 @@
         <v>0</v>
       </c>
     </row>
+    <row r="165" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>99</v>
+      </c>
+      <c r="B165" t="s">
+        <v>100</v>
+      </c>
+      <c r="C165" t="s">
+        <v>101</v>
+      </c>
+      <c r="D165" t="s">
+        <v>101</v>
+      </c>
+      <c r="P165">
+        <v>233</v>
+      </c>
+      <c r="T165">
+        <v>500599.38</v>
+      </c>
+    </row>
+    <row r="166" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>275</v>
+      </c>
+      <c r="B166" t="s">
+        <v>276</v>
+      </c>
+      <c r="C166" t="s">
+        <v>277</v>
+      </c>
+      <c r="D166" t="s">
+        <v>277</v>
+      </c>
+      <c r="P166">
+        <v>128</v>
+      </c>
+      <c r="T166">
+        <v>479571.23</v>
+      </c>
+    </row>
+    <row r="167" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>83</v>
+      </c>
+      <c r="B167" t="s">
+        <v>84</v>
+      </c>
+      <c r="C167" t="s">
+        <v>85</v>
+      </c>
+      <c r="D167" t="s">
+        <v>85</v>
+      </c>
+      <c r="P167">
+        <v>47</v>
+      </c>
+      <c r="T167">
+        <v>323621.26</v>
+      </c>
+    </row>
+    <row r="168" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>359</v>
+      </c>
+      <c r="B168" t="s">
+        <v>360</v>
+      </c>
+      <c r="C168" t="s">
+        <v>361</v>
+      </c>
+      <c r="D168" t="s">
+        <v>361</v>
+      </c>
+      <c r="P168">
+        <v>45</v>
+      </c>
+      <c r="T168">
+        <v>131916.88</v>
+      </c>
+    </row>
+    <row r="169" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>23</v>
+      </c>
+      <c r="B169" t="s">
+        <v>24</v>
+      </c>
+      <c r="C169" t="s">
+        <v>25</v>
+      </c>
+      <c r="D169" t="s">
+        <v>25</v>
+      </c>
+      <c r="P169">
+        <v>66</v>
+      </c>
+      <c r="T169">
+        <v>106554.09</v>
+      </c>
+    </row>
+    <row r="170" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>187</v>
+      </c>
+      <c r="B170" t="s">
+        <v>188</v>
+      </c>
+      <c r="C170" t="s">
+        <v>189</v>
+      </c>
+      <c r="D170" t="s">
+        <v>189</v>
+      </c>
+      <c r="P170">
+        <v>14</v>
+      </c>
+      <c r="T170">
+        <v>66598.37</v>
+      </c>
+    </row>
+    <row r="171" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>171</v>
+      </c>
+      <c r="B171" t="s">
+        <v>172</v>
+      </c>
+      <c r="C171" t="s">
+        <v>173</v>
+      </c>
+      <c r="D171" t="s">
+        <v>173</v>
+      </c>
+      <c r="P171">
+        <v>21</v>
+      </c>
+      <c r="T171">
+        <v>62439.85</v>
+      </c>
+    </row>
+    <row r="172" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>335</v>
+      </c>
+      <c r="B172" t="s">
+        <v>336</v>
+      </c>
+      <c r="C172" t="s">
+        <v>337</v>
+      </c>
+      <c r="D172" t="s">
+        <v>337</v>
+      </c>
+      <c r="P172">
+        <v>19</v>
+      </c>
+      <c r="T172">
+        <v>48320.46</v>
+      </c>
+    </row>
+    <row r="173" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>343</v>
+      </c>
+      <c r="B173" t="s">
+        <v>344</v>
+      </c>
+      <c r="C173" t="s">
+        <v>345</v>
+      </c>
+      <c r="D173" t="s">
+        <v>345</v>
+      </c>
+      <c r="P173">
+        <v>46</v>
+      </c>
+      <c r="T173">
+        <v>44418.67</v>
+      </c>
+    </row>
+    <row r="174" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>51</v>
+      </c>
+      <c r="B174" t="s">
+        <v>52</v>
+      </c>
+      <c r="C174" t="s">
+        <v>53</v>
+      </c>
+      <c r="D174" t="s">
+        <v>53</v>
+      </c>
+      <c r="P174">
+        <v>12</v>
+      </c>
+      <c r="T174">
+        <v>37692.400000000001</v>
+      </c>
+    </row>
+    <row r="175" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>147</v>
+      </c>
+      <c r="B175" t="s">
+        <v>148</v>
+      </c>
+      <c r="C175" t="s">
+        <v>149</v>
+      </c>
+      <c r="D175" t="s">
+        <v>149</v>
+      </c>
+      <c r="P175">
+        <v>73</v>
+      </c>
+      <c r="T175">
+        <v>37375.49</v>
+      </c>
+    </row>
+    <row r="176" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>231</v>
+      </c>
+      <c r="B176" t="s">
+        <v>232</v>
+      </c>
+      <c r="C176" t="s">
+        <v>233</v>
+      </c>
+      <c r="D176" t="s">
+        <v>233</v>
+      </c>
+      <c r="P176">
+        <v>12</v>
+      </c>
+      <c r="T176">
+        <v>36918.65</v>
+      </c>
+    </row>
+    <row r="177" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>111</v>
+      </c>
+      <c r="B177" t="s">
+        <v>112</v>
+      </c>
+      <c r="C177" t="s">
+        <v>113</v>
+      </c>
+      <c r="D177" t="s">
+        <v>113</v>
+      </c>
+      <c r="P177">
+        <v>17</v>
+      </c>
+      <c r="T177">
+        <v>34350.019999999997</v>
+      </c>
+    </row>
+    <row r="178" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>87</v>
+      </c>
+      <c r="B178" t="s">
+        <v>88</v>
+      </c>
+      <c r="C178" t="s">
+        <v>89</v>
+      </c>
+      <c r="D178" t="s">
+        <v>89</v>
+      </c>
+      <c r="P178">
+        <v>3</v>
+      </c>
+      <c r="T178">
+        <v>33811.019999999997</v>
+      </c>
+    </row>
+    <row r="179" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>63</v>
+      </c>
+      <c r="B179" t="s">
+        <v>64</v>
+      </c>
+      <c r="C179" t="s">
+        <v>65</v>
+      </c>
+      <c r="D179" t="s">
+        <v>65</v>
+      </c>
+      <c r="P179">
+        <v>4</v>
+      </c>
+      <c r="T179">
+        <v>32623.73</v>
+      </c>
+    </row>
+    <row r="180" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>103</v>
+      </c>
+      <c r="B180" t="s">
+        <v>104</v>
+      </c>
+      <c r="C180" t="s">
+        <v>105</v>
+      </c>
+      <c r="D180" t="s">
+        <v>105</v>
+      </c>
+      <c r="P180">
+        <v>25</v>
+      </c>
+      <c r="T180">
+        <v>30777.96</v>
+      </c>
+    </row>
+    <row r="181" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>211</v>
+      </c>
+      <c r="B181" t="s">
+        <v>212</v>
+      </c>
+      <c r="C181" t="s">
+        <v>213</v>
+      </c>
+      <c r="D181" t="s">
+        <v>213</v>
+      </c>
+      <c r="P181">
+        <v>26</v>
+      </c>
+      <c r="T181">
+        <v>30435.5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>191</v>
+      </c>
+      <c r="B182" t="s">
+        <v>192</v>
+      </c>
+      <c r="C182" t="s">
+        <v>193</v>
+      </c>
+      <c r="D182" t="s">
+        <v>193</v>
+      </c>
+      <c r="P182">
+        <v>2</v>
+      </c>
+      <c r="T182">
+        <v>22371.18</v>
+      </c>
+    </row>
+    <row r="183" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>339</v>
+      </c>
+      <c r="B183" t="s">
+        <v>340</v>
+      </c>
+      <c r="C183" t="s">
+        <v>341</v>
+      </c>
+      <c r="D183" t="s">
+        <v>341</v>
+      </c>
+      <c r="P183">
+        <v>18</v>
+      </c>
+      <c r="T183">
+        <v>21682.16</v>
+      </c>
+    </row>
+    <row r="184" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>79</v>
+      </c>
+      <c r="B184" t="s">
+        <v>80</v>
+      </c>
+      <c r="C184" t="s">
+        <v>81</v>
+      </c>
+      <c r="D184" t="s">
+        <v>81</v>
+      </c>
+      <c r="P184">
+        <v>53</v>
+      </c>
+      <c r="T184">
+        <v>21624.66</v>
+      </c>
+    </row>
+    <row r="185" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>347</v>
+      </c>
+      <c r="B185" t="s">
+        <v>348</v>
+      </c>
+      <c r="C185" t="s">
+        <v>349</v>
+      </c>
+      <c r="D185" t="s">
+        <v>349</v>
+      </c>
+      <c r="P185">
+        <v>5</v>
+      </c>
+      <c r="T185">
+        <v>19382.189999999999</v>
+      </c>
+    </row>
+    <row r="186" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>143</v>
+      </c>
+      <c r="B186" t="s">
+        <v>144</v>
+      </c>
+      <c r="C186" t="s">
+        <v>145</v>
+      </c>
+      <c r="D186" t="s">
+        <v>145</v>
+      </c>
+      <c r="P186">
+        <v>6</v>
+      </c>
+      <c r="T186">
+        <v>19062.72</v>
+      </c>
+    </row>
+    <row r="187" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>263</v>
+      </c>
+      <c r="B187" t="s">
+        <v>264</v>
+      </c>
+      <c r="C187" t="s">
+        <v>265</v>
+      </c>
+      <c r="D187" t="s">
+        <v>265</v>
+      </c>
+      <c r="P187">
+        <v>9</v>
+      </c>
+      <c r="T187">
+        <v>17239.84</v>
+      </c>
+    </row>
+    <row r="188" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>243</v>
+      </c>
+      <c r="B188" t="s">
+        <v>244</v>
+      </c>
+      <c r="C188" t="s">
+        <v>245</v>
+      </c>
+      <c r="D188" t="s">
+        <v>245</v>
+      </c>
+      <c r="P188">
+        <v>5</v>
+      </c>
+      <c r="T188">
+        <v>16097.47</v>
+      </c>
+    </row>
+    <row r="189" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>251</v>
+      </c>
+      <c r="B189" t="s">
+        <v>252</v>
+      </c>
+      <c r="C189" t="s">
+        <v>253</v>
+      </c>
+      <c r="D189" t="s">
+        <v>253</v>
+      </c>
+      <c r="P189">
+        <v>9</v>
+      </c>
+      <c r="T189">
+        <v>15755.08</v>
+      </c>
+    </row>
+    <row r="190" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>434</v>
+      </c>
+      <c r="B190" t="s">
+        <v>435</v>
+      </c>
+      <c r="C190" t="s">
+        <v>436</v>
+      </c>
+      <c r="D190" t="s">
+        <v>436</v>
+      </c>
+      <c r="P190">
+        <v>9</v>
+      </c>
+      <c r="T190">
+        <v>14483.88</v>
+      </c>
+    </row>
+    <row r="191" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>259</v>
+      </c>
+      <c r="B191" t="s">
+        <v>260</v>
+      </c>
+      <c r="C191" t="s">
+        <v>261</v>
+      </c>
+      <c r="D191" t="s">
+        <v>261</v>
+      </c>
+      <c r="P191">
+        <v>7</v>
+      </c>
+      <c r="T191">
+        <v>14376.29</v>
+      </c>
+    </row>
+    <row r="192" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>367</v>
+      </c>
+      <c r="B192" t="s">
+        <v>368</v>
+      </c>
+      <c r="C192" t="s">
+        <v>369</v>
+      </c>
+      <c r="D192" t="s">
+        <v>369</v>
+      </c>
+      <c r="P192">
+        <v>5</v>
+      </c>
+      <c r="T192">
+        <v>14341.81</v>
+      </c>
+    </row>
+    <row r="193" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>375</v>
+      </c>
+      <c r="B193" t="s">
+        <v>376</v>
+      </c>
+      <c r="C193" t="s">
+        <v>377</v>
+      </c>
+      <c r="D193" t="s">
+        <v>377</v>
+      </c>
+      <c r="P193">
+        <v>3</v>
+      </c>
+      <c r="T193">
+        <v>12709.32</v>
+      </c>
+    </row>
+    <row r="194" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>379</v>
+      </c>
+      <c r="B194" t="s">
+        <v>380</v>
+      </c>
+      <c r="C194" t="s">
+        <v>381</v>
+      </c>
+      <c r="D194" t="s">
+        <v>381</v>
+      </c>
+      <c r="P194">
+        <v>5</v>
+      </c>
+      <c r="T194">
+        <v>12199.16</v>
+      </c>
+    </row>
+    <row r="195" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>235</v>
+      </c>
+      <c r="B195" t="s">
+        <v>236</v>
+      </c>
+      <c r="C195" t="s">
+        <v>237</v>
+      </c>
+      <c r="D195" t="s">
+        <v>237</v>
+      </c>
+      <c r="P195">
+        <v>3</v>
+      </c>
+      <c r="T195">
+        <v>11861.86</v>
+      </c>
+    </row>
+    <row r="196" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>199</v>
+      </c>
+      <c r="B196" t="s">
+        <v>200</v>
+      </c>
+      <c r="C196" t="s">
+        <v>201</v>
+      </c>
+      <c r="D196" t="s">
+        <v>201</v>
+      </c>
+      <c r="P196">
+        <v>6</v>
+      </c>
+      <c r="T196">
+        <v>9740.66</v>
+      </c>
+    </row>
+    <row r="197" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>207</v>
+      </c>
+      <c r="B197" t="s">
+        <v>208</v>
+      </c>
+      <c r="C197" t="s">
+        <v>209</v>
+      </c>
+      <c r="D197" t="s">
+        <v>209</v>
+      </c>
+      <c r="P197">
+        <v>6</v>
+      </c>
+      <c r="T197">
+        <v>9655.92</v>
+      </c>
+    </row>
+    <row r="198" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>247</v>
+      </c>
+      <c r="B198" t="s">
+        <v>248</v>
+      </c>
+      <c r="C198" t="s">
+        <v>249</v>
+      </c>
+      <c r="D198" t="s">
+        <v>249</v>
+      </c>
+      <c r="P198">
+        <v>7</v>
+      </c>
+      <c r="T198">
+        <v>9189.02</v>
+      </c>
+    </row>
+    <row r="199" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>299</v>
+      </c>
+      <c r="B199" t="s">
+        <v>300</v>
+      </c>
+      <c r="C199" t="s">
+        <v>301</v>
+      </c>
+      <c r="D199" t="s">
+        <v>301</v>
+      </c>
+      <c r="P199">
+        <v>3</v>
+      </c>
+      <c r="T199">
+        <v>8834.76</v>
+      </c>
+    </row>
+    <row r="200" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>255</v>
+      </c>
+      <c r="B200" t="s">
+        <v>256</v>
+      </c>
+      <c r="C200" t="s">
+        <v>257</v>
+      </c>
+      <c r="D200" t="s">
+        <v>257</v>
+      </c>
+      <c r="P200">
+        <v>12</v>
+      </c>
+      <c r="T200">
+        <v>8684.7800000000007</v>
+      </c>
+    </row>
+    <row r="201" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>321</v>
+      </c>
+      <c r="B201" t="s">
+        <v>322</v>
+      </c>
+      <c r="C201" t="s">
+        <v>323</v>
+      </c>
+      <c r="D201" t="s">
+        <v>323</v>
+      </c>
+      <c r="P201">
+        <v>3</v>
+      </c>
+      <c r="T201">
+        <v>8556.77</v>
+      </c>
+    </row>
+    <row r="202" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>175</v>
+      </c>
+      <c r="B202" t="s">
+        <v>176</v>
+      </c>
+      <c r="C202" t="s">
+        <v>177</v>
+      </c>
+      <c r="D202" t="s">
+        <v>177</v>
+      </c>
+      <c r="P202">
+        <v>3</v>
+      </c>
+      <c r="T202">
+        <v>8387.2800000000007</v>
+      </c>
+    </row>
+    <row r="203" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>363</v>
+      </c>
+      <c r="B203" t="s">
+        <v>364</v>
+      </c>
+      <c r="C203" t="s">
+        <v>365</v>
+      </c>
+      <c r="D203" t="s">
+        <v>365</v>
+      </c>
+      <c r="P203">
+        <v>2</v>
+      </c>
+      <c r="T203">
+        <v>8303.39</v>
+      </c>
+    </row>
+    <row r="204" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>119</v>
+      </c>
+      <c r="B204" t="s">
+        <v>120</v>
+      </c>
+      <c r="C204" t="s">
+        <v>121</v>
+      </c>
+      <c r="D204" t="s">
+        <v>121</v>
+      </c>
+      <c r="P204">
+        <v>2</v>
+      </c>
+      <c r="T204">
+        <v>8303.39</v>
+      </c>
+    </row>
+    <row r="205" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>331</v>
+      </c>
+      <c r="B205" t="s">
+        <v>332</v>
+      </c>
+      <c r="C205" t="s">
+        <v>333</v>
+      </c>
+      <c r="D205" t="s">
+        <v>333</v>
+      </c>
+      <c r="P205">
+        <v>2</v>
+      </c>
+      <c r="T205">
+        <v>8049.16</v>
+      </c>
+    </row>
+    <row r="206" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>179</v>
+      </c>
+      <c r="B206" t="s">
+        <v>180</v>
+      </c>
+      <c r="C206" t="s">
+        <v>181</v>
+      </c>
+      <c r="D206" t="s">
+        <v>181</v>
+      </c>
+      <c r="P206">
+        <v>3</v>
+      </c>
+      <c r="T206">
+        <v>7861.86</v>
+      </c>
+    </row>
+    <row r="207" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>390</v>
+      </c>
+      <c r="B207" t="s">
+        <v>391</v>
+      </c>
+      <c r="C207" t="s">
+        <v>392</v>
+      </c>
+      <c r="D207" t="s">
+        <v>392</v>
+      </c>
+      <c r="P207">
+        <v>1</v>
+      </c>
+      <c r="T207">
+        <v>7363.56</v>
+      </c>
+    </row>
+    <row r="208" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>311</v>
+      </c>
+      <c r="B208" t="s">
+        <v>312</v>
+      </c>
+      <c r="C208" t="s">
+        <v>313</v>
+      </c>
+      <c r="D208" t="s">
+        <v>313</v>
+      </c>
+      <c r="P208">
+        <v>4</v>
+      </c>
+      <c r="T208">
+        <v>6945.76</v>
+      </c>
+    </row>
+    <row r="209" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>426</v>
+      </c>
+      <c r="B209" t="s">
+        <v>427</v>
+      </c>
+      <c r="C209" t="s">
+        <v>428</v>
+      </c>
+      <c r="D209" t="s">
+        <v>428</v>
+      </c>
+      <c r="P209">
+        <v>2</v>
+      </c>
+      <c r="T209">
+        <v>6693.22</v>
+      </c>
+    </row>
+    <row r="210" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>371</v>
+      </c>
+      <c r="B210" t="s">
+        <v>372</v>
+      </c>
+      <c r="C210" t="s">
+        <v>373</v>
+      </c>
+      <c r="D210" t="s">
+        <v>373</v>
+      </c>
+      <c r="P210">
+        <v>2</v>
+      </c>
+      <c r="T210">
+        <v>6593.22</v>
+      </c>
+    </row>
+    <row r="211" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>386</v>
+      </c>
+      <c r="B211" t="s">
+        <v>387</v>
+      </c>
+      <c r="C211" t="s">
+        <v>388</v>
+      </c>
+      <c r="D211" t="s">
+        <v>388</v>
+      </c>
+      <c r="P211">
+        <v>2</v>
+      </c>
+      <c r="T211">
+        <v>6354.24</v>
+      </c>
+    </row>
+    <row r="212" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>462</v>
+      </c>
+      <c r="B212" t="s">
+        <v>463</v>
+      </c>
+      <c r="C212" t="s">
+        <v>464</v>
+      </c>
+      <c r="D212" t="s">
+        <v>464</v>
+      </c>
+      <c r="P212">
+        <v>1</v>
+      </c>
+      <c r="T212">
+        <v>6016.1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>167</v>
+      </c>
+      <c r="B213" t="s">
+        <v>168</v>
+      </c>
+      <c r="C213" t="s">
+        <v>169</v>
+      </c>
+      <c r="D213" t="s">
+        <v>169</v>
+      </c>
+      <c r="P213">
+        <v>2</v>
+      </c>
+      <c r="T213">
+        <v>6015.25</v>
+      </c>
+    </row>
+    <row r="214" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>183</v>
+      </c>
+      <c r="B214" t="s">
+        <v>184</v>
+      </c>
+      <c r="C214" t="s">
+        <v>185</v>
+      </c>
+      <c r="D214" t="s">
+        <v>185</v>
+      </c>
+      <c r="P214">
+        <v>2</v>
+      </c>
+      <c r="T214">
+        <v>5761.02</v>
+      </c>
+    </row>
+    <row r="215" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>317</v>
+      </c>
+      <c r="B215" t="s">
+        <v>318</v>
+      </c>
+      <c r="C215" t="s">
+        <v>319</v>
+      </c>
+      <c r="D215" t="s">
+        <v>319</v>
+      </c>
+      <c r="P215">
+        <v>10</v>
+      </c>
+      <c r="T215">
+        <v>5737.29</v>
+      </c>
+    </row>
+    <row r="216" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>303</v>
+      </c>
+      <c r="B216" t="s">
+        <v>304</v>
+      </c>
+      <c r="C216" t="s">
+        <v>305</v>
+      </c>
+      <c r="D216" t="s">
+        <v>305</v>
+      </c>
+      <c r="P216">
+        <v>4</v>
+      </c>
+      <c r="T216">
+        <v>5420.32</v>
+      </c>
+    </row>
+    <row r="217" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>414</v>
+      </c>
+      <c r="B217" t="s">
+        <v>415</v>
+      </c>
+      <c r="C217" t="s">
+        <v>416</v>
+      </c>
+      <c r="D217" t="s">
+        <v>416</v>
+      </c>
+      <c r="P217">
+        <v>1</v>
+      </c>
+      <c r="T217">
+        <v>5390.56</v>
+      </c>
+    </row>
+    <row r="218" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>383</v>
+      </c>
+      <c r="B218" t="s">
+        <v>48</v>
+      </c>
+      <c r="C218" t="s">
+        <v>384</v>
+      </c>
+      <c r="D218" t="s">
+        <v>384</v>
+      </c>
+      <c r="P218">
+        <v>5</v>
+      </c>
+      <c r="T218">
+        <v>5165.25</v>
+      </c>
+    </row>
+    <row r="219" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>59</v>
+      </c>
+      <c r="B219" t="s">
+        <v>60</v>
+      </c>
+      <c r="C219" t="s">
+        <v>61</v>
+      </c>
+      <c r="D219" t="s">
+        <v>61</v>
+      </c>
+      <c r="P219">
+        <v>5</v>
+      </c>
+      <c r="T219">
+        <v>4961.8500000000004</v>
+      </c>
+    </row>
+    <row r="220" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>215</v>
+      </c>
+      <c r="B220" t="s">
+        <v>216</v>
+      </c>
+      <c r="C220" t="s">
+        <v>217</v>
+      </c>
+      <c r="D220" t="s">
+        <v>217</v>
+      </c>
+      <c r="P220">
+        <v>12</v>
+      </c>
+      <c r="T220">
+        <v>4379.66</v>
+      </c>
+    </row>
+    <row r="221" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>71</v>
+      </c>
+      <c r="B221" t="s">
+        <v>72</v>
+      </c>
+      <c r="C221" t="s">
+        <v>73</v>
+      </c>
+      <c r="D221" t="s">
+        <v>73</v>
+      </c>
+      <c r="P221">
+        <v>3</v>
+      </c>
+      <c r="T221">
+        <v>4268.6400000000003</v>
+      </c>
+    </row>
+    <row r="222" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>327</v>
+      </c>
+      <c r="B222" t="s">
+        <v>328</v>
+      </c>
+      <c r="C222" t="s">
+        <v>329</v>
+      </c>
+      <c r="D222" t="s">
+        <v>329</v>
+      </c>
+      <c r="P222">
+        <v>7</v>
+      </c>
+      <c r="T222">
+        <v>4211.84</v>
+      </c>
+    </row>
+    <row r="223" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>163</v>
+      </c>
+      <c r="B223" t="s">
+        <v>164</v>
+      </c>
+      <c r="C223" t="s">
+        <v>165</v>
+      </c>
+      <c r="D223" t="s">
+        <v>165</v>
+      </c>
+      <c r="P223">
+        <v>4</v>
+      </c>
+      <c r="T223">
+        <v>4106.7700000000004</v>
+      </c>
+    </row>
+    <row r="224" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>406</v>
+      </c>
+      <c r="B224" t="s">
+        <v>407</v>
+      </c>
+      <c r="C224" t="s">
+        <v>408</v>
+      </c>
+      <c r="D224" t="s">
+        <v>408</v>
+      </c>
+      <c r="P224">
+        <v>1</v>
+      </c>
+      <c r="T224">
+        <v>4079.42</v>
+      </c>
+    </row>
+    <row r="225" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>239</v>
+      </c>
+      <c r="B225" t="s">
+        <v>240</v>
+      </c>
+      <c r="C225" t="s">
+        <v>241</v>
+      </c>
+      <c r="D225" t="s">
+        <v>241</v>
+      </c>
+      <c r="P225">
+        <v>2</v>
+      </c>
+      <c r="T225">
+        <v>3218.64</v>
+      </c>
+    </row>
+    <row r="226" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>203</v>
+      </c>
+      <c r="B226" t="s">
+        <v>204</v>
+      </c>
+      <c r="C226" t="s">
+        <v>205</v>
+      </c>
+      <c r="D226" t="s">
+        <v>205</v>
+      </c>
+      <c r="P226">
+        <v>1</v>
+      </c>
+      <c r="T226">
+        <v>2895.91</v>
+      </c>
+    </row>
+    <row r="227" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>131</v>
+      </c>
+      <c r="B227" t="s">
+        <v>132</v>
+      </c>
+      <c r="C227" t="s">
+        <v>133</v>
+      </c>
+      <c r="D227" t="s">
+        <v>133</v>
+      </c>
+      <c r="P227">
+        <v>1</v>
+      </c>
+      <c r="T227">
+        <v>2824.58</v>
+      </c>
+    </row>
+    <row r="228" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>459</v>
+      </c>
+      <c r="B228" t="s">
+        <v>128</v>
+      </c>
+      <c r="C228" t="s">
+        <v>460</v>
+      </c>
+      <c r="D228" t="s">
+        <v>460</v>
+      </c>
+      <c r="P228">
+        <v>1</v>
+      </c>
+      <c r="T228">
+        <v>2357.06</v>
+      </c>
+    </row>
+    <row r="229" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>139</v>
+      </c>
+      <c r="B229" t="s">
+        <v>140</v>
+      </c>
+      <c r="C229" t="s">
+        <v>141</v>
+      </c>
+      <c r="D229" t="s">
+        <v>141</v>
+      </c>
+      <c r="P229">
+        <v>6</v>
+      </c>
+      <c r="T229">
+        <v>2283.04</v>
+      </c>
+    </row>
+    <row r="230" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>307</v>
+      </c>
+      <c r="B230" t="s">
+        <v>308</v>
+      </c>
+      <c r="C230" t="s">
+        <v>309</v>
+      </c>
+      <c r="D230" t="s">
+        <v>309</v>
+      </c>
+      <c r="P230">
+        <v>1</v>
+      </c>
+      <c r="T230">
+        <v>2117.8000000000002</v>
+      </c>
+    </row>
+    <row r="231" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>325</v>
+      </c>
+      <c r="B231" t="s">
+        <v>92</v>
+      </c>
+      <c r="C231" t="s">
+        <v>326</v>
+      </c>
+      <c r="D231" t="s">
+        <v>326</v>
+      </c>
+      <c r="P231">
+        <v>1</v>
+      </c>
+      <c r="T231">
+        <v>1738.22</v>
+      </c>
+    </row>
+    <row r="232" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>457</v>
+      </c>
+      <c r="B232" t="s">
+        <v>224</v>
+      </c>
+      <c r="C232" t="s">
+        <v>458</v>
+      </c>
+      <c r="D232" t="s">
+        <v>458</v>
+      </c>
+      <c r="P232">
+        <v>1</v>
+      </c>
+      <c r="T232">
+        <v>1685.59</v>
+      </c>
+    </row>
+    <row r="233" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>43</v>
+      </c>
+      <c r="B233" t="s">
+        <v>44</v>
+      </c>
+      <c r="C233" t="s">
+        <v>45</v>
+      </c>
+      <c r="D233" t="s">
+        <v>45</v>
+      </c>
+      <c r="P233">
+        <v>1</v>
+      </c>
+      <c r="T233">
+        <v>1663.56</v>
+      </c>
+    </row>
+    <row r="234" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>135</v>
+      </c>
+      <c r="B234" t="s">
+        <v>136</v>
+      </c>
+      <c r="C234" t="s">
+        <v>137</v>
+      </c>
+      <c r="D234" t="s">
+        <v>137</v>
+      </c>
+      <c r="P234">
+        <v>1</v>
+      </c>
+      <c r="T234">
+        <v>1609.32</v>
+      </c>
+    </row>
+    <row r="235" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>75</v>
+      </c>
+      <c r="B235" t="s">
+        <v>76</v>
+      </c>
+      <c r="C235" t="s">
+        <v>77</v>
+      </c>
+      <c r="D235" t="s">
+        <v>77</v>
+      </c>
+      <c r="P235">
+        <v>1</v>
+      </c>
+      <c r="T235">
+        <v>1483.9</v>
+      </c>
+    </row>
+    <row r="236" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
+        <v>315</v>
+      </c>
+      <c r="B236" t="s">
+        <v>36</v>
+      </c>
+      <c r="C236" t="s">
+        <v>316</v>
+      </c>
+      <c r="D236" t="s">
+        <v>316</v>
+      </c>
+      <c r="P236">
+        <v>1</v>
+      </c>
+      <c r="T236">
+        <v>1312.71</v>
+      </c>
+    </row>
+    <row r="237" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>351</v>
+      </c>
+      <c r="B237" t="s">
+        <v>352</v>
+      </c>
+      <c r="C237" t="s">
+        <v>353</v>
+      </c>
+      <c r="D237" t="s">
+        <v>353</v>
+      </c>
+      <c r="P237">
+        <v>1</v>
+      </c>
+      <c r="T237">
+        <v>1092.3699999999999</v>
+      </c>
+    </row>
+    <row r="238" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>271</v>
+      </c>
+      <c r="B238" t="s">
+        <v>272</v>
+      </c>
+      <c r="C238" t="s">
+        <v>273</v>
+      </c>
+      <c r="D238" t="s">
+        <v>273</v>
+      </c>
+      <c r="P238">
+        <v>1</v>
+      </c>
+      <c r="T238">
+        <v>1083.9000000000001</v>
+      </c>
+    </row>
+    <row r="239" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
+        <v>398</v>
+      </c>
+      <c r="B239" t="s">
+        <v>399</v>
+      </c>
+      <c r="C239" t="s">
+        <v>400</v>
+      </c>
+      <c r="D239" t="s">
+        <v>400</v>
+      </c>
+      <c r="P239">
+        <v>0</v>
+      </c>
+      <c r="T239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
+        <v>123</v>
+      </c>
+      <c r="B240" t="s">
+        <v>124</v>
+      </c>
+      <c r="C240" t="s">
+        <v>125</v>
+      </c>
+      <c r="D240" t="s">
+        <v>125</v>
+      </c>
+      <c r="P240">
+        <v>0</v>
+      </c>
+      <c r="T240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
+        <v>55</v>
+      </c>
+      <c r="B241" t="s">
+        <v>56</v>
+      </c>
+      <c r="C241" t="s">
+        <v>57</v>
+      </c>
+      <c r="D241" t="s">
+        <v>57</v>
+      </c>
+      <c r="P241">
+        <v>0</v>
+      </c>
+      <c r="T241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
+        <v>115</v>
+      </c>
+      <c r="B242" t="s">
+        <v>116</v>
+      </c>
+      <c r="C242" t="s">
+        <v>117</v>
+      </c>
+      <c r="D242" t="s">
+        <v>117</v>
+      </c>
+      <c r="P242">
+        <v>0</v>
+      </c>
+      <c r="T242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
+        <v>27</v>
+      </c>
+      <c r="B243" t="s">
+        <v>28</v>
+      </c>
+      <c r="C243" t="s">
+        <v>29</v>
+      </c>
+      <c r="D243" t="s">
+        <v>29</v>
+      </c>
+      <c r="P243">
+        <v>0</v>
+      </c>
+      <c r="T243">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>